<commit_message>
UI: mover sección encima del enunciado y ocultar '(Puntuación: X)' en opciones. Fix: reemplazo de Excel inválido (.xlsx) y verificación de carga. Docs: indicaciones de rerun/clear cache en Streamlit.
</commit_message>
<xml_diff>
--- a/data/Cuestionario de autodiagnóstico en inclusión laboral LGBTIQ para agencias de empleo..xlsx
+++ b/data/Cuestionario de autodiagnóstico en inclusión laboral LGBTIQ para agencias de empleo..xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcgm/Desktop/Gpt- LGBTIQ+/ExcelInteractivo/mi_app_inclusiva/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C1F7F-9BE8-46CC-9B0D-B11D8F43EAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9299F-32F9-394B-889D-EC9F38B209EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="9" r:id="rId1"/>
@@ -610,9 +610,6 @@
     <t>Al finalizar, el puntaje total ubicará a su Agencia de Empleo, en uno de los tres niveles: Inicial, Intermedio o Avanzado.</t>
   </si>
   <si>
-    <t>¿En los protocolos de la Agencia, garantiza el reconocimiento y uso del nombre identitario y pronombres de las personas LGBTIQ+ en todos los procesos internos y externos relacionados con la vinculación y gestión del talento?</t>
-  </si>
-  <si>
     <t>¿Actualmente, cuenta con protocolos formales que garanticen el trato digno, respetuoso y libre de discriminación hacia personas LGBTIQ+ en todos los procesos de gestión del talento humano?</t>
   </si>
   <si>
@@ -632,6 +629,9 @@
   </si>
   <si>
     <t>Se cuenta con un enfoque diferencial LGBTIQ+ consolidado, transversal e institucionalizado, respaldado por políticas, procedimientos y acciones coordinadas que se aplican de forma consistente en todos los procesos.</t>
+  </si>
+  <si>
+    <t>¿En los protocolos de la Agencia o Bolsa de empleo, se garantiza el reconocimiento y uso del nombre identitario y pronombres de las personas LGBTIQ+ en todos los procesos internos y externos relacionados con la vinculación y gestión del talento?</t>
   </si>
 </sst>
 </file>
@@ -989,6 +989,18 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1063,18 +1075,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2754,26 +2754,26 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="25"/>
-    <col min="2" max="2" width="153.7109375" style="27" customWidth="1"/>
-    <col min="3" max="11" width="11.42578125" style="25"/>
-    <col min="12" max="12" width="51.140625" style="25" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="25"/>
+    <col min="1" max="1" width="11.5" style="25"/>
+    <col min="2" max="2" width="153.6640625" style="27" customWidth="1"/>
+    <col min="3" max="11" width="11.5" style="25"/>
+    <col min="12" max="12" width="51.1640625" style="25" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="40"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40"/>
-    </row>
-    <row r="3" spans="1:11" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
+    <row r="1" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="44"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="43" t="s">
         <v>112</v>
       </c>
       <c r="C5" s="24"/>
@@ -2786,8 +2786,8 @@
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="43"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -2798,22 +2798,22 @@
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="B8" s="27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="B9" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="B11" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="26">
         <v>1</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="26">
         <v>2</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="26">
         <v>3</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="26">
         <v>4</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="26">
         <v>5</v>
       </c>
@@ -2853,24 +2853,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="26"/>
       <c r="B17" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B19" s="28"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="B20" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="B21" s="27" t="s">
         <v>42</v>
       </c>
@@ -2889,103 +2889,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D3059B-A79D-48BC-B93F-134A67344FC0}">
   <dimension ref="B1:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="5.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="3"/>
+    <col min="2" max="2" width="5.5" style="9" customWidth="1"/>
     <col min="3" max="3" width="99" style="14" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="11.5" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-    </row>
-    <row r="2" spans="2:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-    </row>
-    <row r="3" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+    <row r="1" spans="2:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+    </row>
+    <row r="2" spans="2:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+    </row>
+    <row r="3" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:8" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="54" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+    </row>
+    <row r="6" spans="2:8" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C7" s="9"/>
     </row>
-    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="51"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="42" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="42">
+        <v>161</v>
+      </c>
+      <c r="D10" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="28" x14ac:dyDescent="0.2">
       <c r="B11" s="11">
         <v>3</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="43"/>
-    </row>
-    <row r="12" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="D11" s="47"/>
+    </row>
+    <row r="12" spans="2:8" ht="28" x14ac:dyDescent="0.2">
       <c r="B12" s="11">
         <v>2</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="43"/>
-    </row>
-    <row r="13" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="D12" s="47"/>
+    </row>
+    <row r="13" spans="2:8" ht="28" x14ac:dyDescent="0.2">
       <c r="B13" s="11">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="44"/>
-    </row>
-    <row r="16" spans="2:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="s">
+      <c r="D13" s="48"/>
+    </row>
+    <row r="16" spans="2:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="53"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="10" t="s">
         <v>2</v>
       </c>
@@ -2994,421 +2994,421 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="42">
+        <v>154</v>
+      </c>
+      <c r="D17" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B18" s="11">
         <v>3</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="43"/>
-    </row>
-    <row r="19" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D18" s="47"/>
+    </row>
+    <row r="19" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B19" s="11">
         <v>2</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="43"/>
-    </row>
-    <row r="20" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D19" s="47"/>
+    </row>
+    <row r="20" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B20" s="11">
         <v>1</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="44"/>
-    </row>
-    <row r="23" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47" t="s">
+      <c r="D20" s="48"/>
+    </row>
+    <row r="23" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="47"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="42">
+        <v>155</v>
+      </c>
+      <c r="D24" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B25" s="11">
         <v>3</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="43"/>
-    </row>
-    <row r="26" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D25" s="47"/>
+    </row>
+    <row r="26" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B26" s="11">
         <v>2</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="43"/>
-    </row>
-    <row r="27" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D26" s="47"/>
+    </row>
+    <row r="27" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B27" s="11">
         <v>1</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="44"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="47" t="s">
+      <c r="D27" s="48"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="11">
         <v>3</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="43"/>
-    </row>
-    <row r="33" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D32" s="47"/>
+    </row>
+    <row r="33" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B33" s="11">
         <v>2</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="43"/>
-    </row>
-    <row r="34" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="47"/>
+    </row>
+    <row r="34" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="11">
         <v>1</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="44"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="41" t="s">
+      <c r="D34" s="48"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B37" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="41"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B38" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B39" s="11">
         <v>3</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="43"/>
-    </row>
-    <row r="40" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D39" s="47"/>
+    </row>
+    <row r="40" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B40" s="11">
         <v>2</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="43"/>
-    </row>
-    <row r="41" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D40" s="47"/>
+    </row>
+    <row r="41" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="44"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="48" t="s">
+      <c r="D41" s="48"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="48"/>
+      <c r="C44" s="52"/>
       <c r="D44" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="42">
+        <v>156</v>
+      </c>
+      <c r="D45" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B46" s="19">
         <v>3</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D46" s="43"/>
-    </row>
-    <row r="47" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D46" s="47"/>
+    </row>
+    <row r="47" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B47" s="19">
         <v>2</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="43"/>
-    </row>
-    <row r="48" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D47" s="47"/>
+    </row>
+    <row r="48" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B48" s="19">
         <v>1</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="44"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="41" t="s">
+      <c r="D48" s="48"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B51" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="41"/>
+      <c r="C51" s="45"/>
       <c r="D51" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B52" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D52" s="42">
+        <v>157</v>
+      </c>
+      <c r="D52" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B53" s="11">
         <v>3</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="43"/>
-    </row>
-    <row r="54" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D53" s="47"/>
+    </row>
+    <row r="54" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B54" s="11">
         <v>2</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="43"/>
-    </row>
-    <row r="55" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D54" s="47"/>
+    </row>
+    <row r="55" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B55" s="11">
         <v>1</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="44"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="41" t="s">
+      <c r="D55" s="48"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B58" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="41"/>
+      <c r="C58" s="45"/>
       <c r="D58" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B59" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="42">
+      <c r="D59" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="42" x14ac:dyDescent="0.2">
       <c r="B60" s="11">
         <v>3</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="43"/>
-    </row>
-    <row r="61" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D60" s="47"/>
+    </row>
+    <row r="61" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B61" s="11">
         <v>2</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="43"/>
-    </row>
-    <row r="62" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D61" s="47"/>
+    </row>
+    <row r="62" spans="2:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B62" s="11">
         <v>1</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D62" s="44"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="46" t="s">
+      <c r="D62" s="48"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B65" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="46"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B66" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" s="42">
+        <v>158</v>
+      </c>
+      <c r="D66" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B67" s="19">
         <v>3</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D67" s="43"/>
-    </row>
-    <row r="68" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="D67" s="47"/>
+    </row>
+    <row r="68" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B68" s="19">
         <v>2</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="43"/>
-    </row>
-    <row r="69" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D68" s="47"/>
+    </row>
+    <row r="69" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B69" s="19">
         <v>1</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="44"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="41" t="s">
+      <c r="D69" s="48"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B72" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C72" s="41"/>
+      <c r="C72" s="45"/>
       <c r="D72" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="2:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B73" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="D73" s="42">
+        <v>159</v>
+      </c>
+      <c r="D73" s="46">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B74" s="11">
         <v>3</v>
       </c>
       <c r="C74" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="D74" s="43"/>
-    </row>
-    <row r="75" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D74" s="47"/>
+    </row>
+    <row r="75" spans="2:4" ht="28" x14ac:dyDescent="0.15">
       <c r="B75" s="11">
         <v>2</v>
       </c>
       <c r="C75" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D75" s="43"/>
-    </row>
-    <row r="76" spans="2:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="D75" s="47"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B76" s="11">
         <v>1</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D76" s="44"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="48"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C77" s="12" t="s">
         <v>21</v>
       </c>
@@ -3417,24 +3417,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C78" s="23"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C80" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="45" t="str">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="49" t="str">
         <f>IF(D77&lt;=15,"Nivel 1 – Inicial: Recomendamos ruta 'Brújula Diversa' (ABC de la diversidad; Sesgos inconscientes; Pautas de atención a clientes y usuarios diversos; Lenguaje inclusivo)",
 IF(D77&lt;=23,"Nivel 2 – Intermedio: Recomendamos ruta 'Culturas que cuidan' (Espacios seguros; ABC de orientaciones e identidades; Rompiendo estereotipos; Formación en diversidad para equipos de talento humano)",
 "Nivel 3 – Avanzado: Recomendamos ruta 'Talento sin etiquetas' (Entrevista libre de sesgos; Talento trans; Interseccionalidad; Procesos de contratación desde una mirada jurídica)"))</f>
         <v>Nivel 1 – Inicial: Recomendamos ruta 'Brújula Diversa' (ABC de la diversidad; Sesgos inconscientes; Pautas de atención a clientes y usuarios diversos; Lenguaje inclusivo)</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="45"/>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3529,13 +3529,13 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="29" t="s">
         <v>24</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" ht="112" x14ac:dyDescent="0.2">
       <c r="C3" s="29" t="s">
         <v>26</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="315" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" ht="335" x14ac:dyDescent="0.2">
       <c r="C4" s="29" t="s">
         <v>27</v>
       </c>
@@ -3559,16 +3559,16 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="55" t="s">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="59" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C6" s="56"/>
+    <row r="6" spans="3:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="C6" s="60"/>
       <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
@@ -3592,13 +3592,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="32" t="s">
         <v>24</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="32" t="s">
         <v>26</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="375" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" ht="350" x14ac:dyDescent="0.2">
       <c r="C4" s="32" t="s">
         <v>27</v>
       </c>
@@ -3622,16 +3622,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="57" t="s">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="61" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C6" s="58"/>
+    <row r="6" spans="3:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="C6" s="62"/>
       <c r="D6" s="5" t="s">
         <v>32</v>
       </c>
@@ -3655,13 +3655,13 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="30.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="30" t="s">
         <v>24</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="30" t="s">
         <v>26</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="376.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" ht="376.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="30" t="s">
         <v>27</v>
       </c>
@@ -3685,16 +3685,16 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="59" t="s">
+    <row r="5" spans="3:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C5" s="63" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="C6" s="60"/>
+    <row r="6" spans="3:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="C6" s="64"/>
       <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
@@ -3711,30 +3711,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3E33B8-CEE5-9342-850C-E2B013C57098}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="66" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="65" customWidth="1"/>
-    <col min="3" max="5" width="31" style="65" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" style="65" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="65"/>
+    <col min="1" max="1" width="25.33203125" style="41" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="40" customWidth="1"/>
+    <col min="3" max="5" width="31" style="40" customWidth="1"/>
+    <col min="6" max="6" width="42.5" style="40" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="67" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:6" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
-    </row>
-    <row r="2" spans="1:6" s="67" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
+    </row>
+    <row r="2" spans="1:6" s="42" customFormat="1" ht="38" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>46</v>
       </c>
@@ -3754,203 +3754,203 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="293.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="310.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="293.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="276" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="238" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="258.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="238" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="E8" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="39" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="224.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="39" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="207" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="224.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="207" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="39" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3970,19 +3970,19 @@
       <selection activeCell="F10" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>1</v>
       </c>

</xml_diff>